<commit_message>
calculate the profit margin
</commit_message>
<xml_diff>
--- a/kitchen_supplies_profit.xlsx
+++ b/kitchen_supplies_profit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Projects\Data_Analysis_Portfolio\composite_function\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF910D24-5742-4117-AC90-E430AF0B26E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF4A90D-8CA1-4499-ABBB-7ED9893B469F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Product ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Total Revenue</t>
+  </si>
+  <si>
+    <t>Profit Margin</t>
   </si>
 </sst>
 </file>
@@ -316,10 +319,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -415,12 +418,22 @@
       <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
         <f>SUMPRODUCT(B3:B7, C3:C7)</f>
         <v>655</v>
       </c>
+      <c r="C11" s="4">
+        <f>SUMPRODUCT(B3:B7,C3:C7,D3:D7)</f>
+        <v>156.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>